<commit_message>
Minor fix need more check
</commit_message>
<xml_diff>
--- a/doc/support_Instruction_OP_code.xlsx
+++ b/doc/support_Instruction_OP_code.xlsx
@@ -2,13 +2,13 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\cad_project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66DEFC3E-F9B8-43C1-ABA7-17637A076986}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228AF62A-7B17-4B28-9557-4B3196DFE530}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{22F9996F-6530-4A1E-BC46-DC118D46B476}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="45">
   <si>
     <t>OP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -127,14 +127,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>`00</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>XX</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>X</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -144,14 +136,6 @@
   </si>
   <si>
     <t>x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>xx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>`01</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -291,9 +275,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 佈景主題">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="有機">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="有機">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -301,48 +285,83 @@
         <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546A"/>
+        <a:srgbClr val="212121"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="E7E6E6"/>
+        <a:srgbClr val="DADADA"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472C4"/>
+        <a:srgbClr val="83992A"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ED7D31"/>
+        <a:srgbClr val="3C9770"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="A5A5A5"/>
+        <a:srgbClr val="44709D"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="FFC000"/>
+        <a:srgbClr val="A23C33"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5B9BD5"/>
+        <a:srgbClr val="D97828"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70AD47"/>
+        <a:srgbClr val="DEB340"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563C1"/>
+        <a:srgbClr val="A8BF4D"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954F72"/>
+        <a:srgbClr val="B4CA80"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="有機">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Garamond" panose="02020404030301010803"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック Light"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线 Light"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="돋움"/>
+        <a:font script="Hans" typeface="方正舒体"/>
+        <a:font script="Hant" typeface="微軟正黑體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Garamond" panose="02020404030301010803"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐ明朝"/>
+        <a:font script="Hang" typeface="바탕"/>
+        <a:font script="Hans" typeface="方正舒体"/>
         <a:font script="Hant" typeface="新細明體"/>
         <a:font script="Arab" typeface="Times New Roman"/>
         <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Thai" typeface="Angsana New"/>
         <a:font script="Ethi" typeface="Nyala"/>
         <a:font script="Beng" typeface="Vrinda"/>
         <a:font script="Gujr" typeface="Shruti"/>
@@ -366,78 +385,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="游ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="等线"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="有機">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -446,76 +396,54 @@
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
+                <a:tint val="60000"/>
                 <a:lumMod val="110000"/>
-                <a:satMod val="105000"/>
-                <a:tint val="67000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="103000"/>
-                <a:tint val="73000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:lumMod val="105000"/>
-                <a:satMod val="109000"/>
-                <a:tint val="81000"/>
+                <a:tint val="82000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+            <a:duotone>
               <a:schemeClr val="phClr">
-                <a:satMod val="103000"/>
-                <a:lumMod val="102000"/>
+                <a:shade val="74000"/>
+                <a:satMod val="130000"/>
+                <a:lumMod val="90000"/>
+              </a:schemeClr>
+              <a:schemeClr val="phClr">
                 <a:tint val="94000"/>
+                <a:satMod val="120000"/>
+                <a:lumMod val="104000"/>
               </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:satMod val="110000"/>
-                <a:lumMod val="100000"/>
-                <a:shade val="100000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:lumMod val="99000"/>
-                <a:satMod val="120000"/>
-                <a:shade val="78000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="5400000" scaled="0"/>
-        </a:gradFill>
+            </a:duotone>
+          </a:blip>
+          <a:tile tx="0" ty="0" sx="100000" sy="100000" flip="none" algn="tl"/>
+        </a:blipFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="15875" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="800000"/>
         </a:ln>
       </a:lnStyleLst>
       <a:effectStyleLst>
@@ -523,13 +451,19 @@
           <a:effectLst/>
         </a:effectStyle>
         <a:effectStyle>
-          <a:effectLst/>
+          <a:effectLst>
+            <a:innerShdw blurRad="25400" dist="12700" dir="13500000">
+              <a:srgbClr val="000000">
+                <a:alpha val="45000"/>
+              </a:srgbClr>
+            </a:innerShdw>
+          </a:effectLst>
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw blurRad="38100" dist="25400" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
-                <a:alpha val="63000"/>
+                <a:alpha val="60000"/>
               </a:srgbClr>
             </a:outerShdw>
           </a:effectLst>
@@ -539,39 +473,27 @@
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
-        <a:solidFill>
-          <a:schemeClr val="phClr">
-            <a:tint val="95000"/>
-            <a:satMod val="170000"/>
-          </a:schemeClr>
-        </a:solidFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
             <a:gs pos="0">
               <a:schemeClr val="phClr">
-                <a:tint val="93000"/>
-                <a:satMod val="150000"/>
-                <a:shade val="98000"/>
-                <a:lumMod val="102000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="50000">
-              <a:schemeClr val="phClr">
-                <a:tint val="98000"/>
-                <a:satMod val="130000"/>
-                <a:shade val="90000"/>
-                <a:lumMod val="103000"/>
+                <a:tint val="90000"/>
+                <a:lumMod val="110000"/>
               </a:schemeClr>
             </a:gs>
             <a:gs pos="100000">
               <a:schemeClr val="phClr">
-                <a:shade val="63000"/>
-                <a:satMod val="120000"/>
+                <a:shade val="88000"/>
+                <a:lumMod val="98000"/>
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
         </a:gradFill>
+        <a:blipFill>
+          <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+          <a:stretch/>
+        </a:blipFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
@@ -579,7 +501,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Organic" id="{28CDC826-8792-45C0-861B-85EB3ADEDA33}" vid="{7DAC20F1-423D-49E2-BD0B-50532748BAD0}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -587,10 +509,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCB8D60-9B4B-40ED-B1FB-BD3142EAA964}">
-  <dimension ref="A1:L19"/>
+  <dimension ref="A1:M19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -598,7 +520,7 @@
     <col min="9" max="9" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -618,7 +540,7 @@
         <v>5</v>
       </c>
       <c r="H1" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="I1" t="s">
         <v>7</v>
@@ -630,10 +552,13 @@
         <v>9</v>
       </c>
       <c r="L1" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+        <v>44</v>
+      </c>
+      <c r="M1">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
@@ -643,8 +568,8 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2" t="s">
-        <v>25</v>
+      <c r="D2">
+        <v>0</v>
       </c>
       <c r="E2">
         <v>0</v>
@@ -671,7 +596,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -682,7 +607,7 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -691,7 +616,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -700,16 +625,16 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K3" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>12</v>
       </c>
@@ -720,7 +645,7 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -741,13 +666,13 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>13</v>
       </c>
@@ -757,8 +682,8 @@
       <c r="C5">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
-        <v>31</v>
+      <c r="D5">
+        <v>1</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -785,7 +710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>14</v>
       </c>
@@ -796,7 +721,7 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -823,7 +748,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>15</v>
       </c>
@@ -833,8 +758,8 @@
       <c r="C7">
         <v>0</v>
       </c>
-      <c r="D7" t="s">
-        <v>25</v>
+      <c r="D7">
+        <v>0</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -861,7 +786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -871,8 +796,8 @@
       <c r="C8">
         <v>0</v>
       </c>
-      <c r="D8" t="s">
-        <v>25</v>
+      <c r="D8">
+        <v>0</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -899,7 +824,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>16</v>
       </c>
@@ -909,8 +834,8 @@
       <c r="C9">
         <v>0</v>
       </c>
-      <c r="D9" t="s">
-        <v>25</v>
+      <c r="D9">
+        <v>0</v>
       </c>
       <c r="E9">
         <v>0</v>
@@ -937,18 +862,18 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>44</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -957,7 +882,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -966,27 +891,27 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K10" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L10">
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="B11" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -995,7 +920,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -1004,63 +929,63 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="K11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="L11">
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>29</v>
+      </c>
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+      <c r="D14" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>30</v>
+      </c>
+      <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
+        <v>32</v>
+      </c>
+      <c r="D15" t="s">
         <v>33</v>
       </c>
-      <c r="B14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C14" t="s">
-        <v>36</v>
-      </c>
-      <c r="D14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="E15" t="s">
         <v>34</v>
-      </c>
-      <c r="B15" t="s">
-        <v>29</v>
-      </c>
-      <c r="C15" t="s">
-        <v>36</v>
-      </c>
-      <c r="D15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="B17" t="s">
         <v>10</v>
@@ -1071,10 +996,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="B19" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
CHECKPOINT 2- Processor Done
</commit_message>
<xml_diff>
--- a/doc/support_Instruction_OP_code.xlsx
+++ b/doc/support_Instruction_OP_code.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20391"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20392"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\cad_project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E972F98B-5597-4253-B800-2F3753E52160}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEEBFC5-6AB3-4383-976F-C52D4D87456D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{22F9996F-6530-4A1E-BC46-DC118D46B476}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
   <si>
     <t>OP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -208,6 +208,14 @@
   </si>
   <si>
     <t>stop</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>NOP</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`1111</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -513,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9BCB8D60-9B4B-40ED-B1FB-BD3142EAA964}">
-  <dimension ref="A1:M19"/>
+  <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+      <selection activeCell="A13" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
@@ -973,72 +981,113 @@
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="A12" t="s">
+        <v>46</v>
+      </c>
+      <c r="B12" t="s">
+        <v>47</v>
+      </c>
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="B12" s="1"/>
-      <c r="C12" s="1"/>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
         <v>29</v>
       </c>
-      <c r="B14" t="s">
+      <c r="B17" t="s">
         <v>31</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="D14" t="s">
+      <c r="D17" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>30</v>
       </c>
-      <c r="B15" t="s">
-        <v>27</v>
-      </c>
-      <c r="C15" t="s">
+      <c r="B18" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" t="s">
         <v>32</v>
       </c>
-      <c r="D15" t="s">
+      <c r="D18" t="s">
         <v>33</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E18" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>37</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
         <v>10</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
         <v>38</v>
       </c>
-      <c r="B19" t="s">
+      <c r="B22" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A12:E12"/>
+    <mergeCell ref="A15:E15"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
TEST5_TB done need test
</commit_message>
<xml_diff>
--- a/doc/support_Instruction_OP_code.xlsx
+++ b/doc/support_Instruction_OP_code.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\cad_project\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AEEBFC5-6AB3-4383-976F-C52D4D87456D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3BC9B588-1EDF-4551-95D3-93DF38A10225}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12180" xr2:uid="{22F9996F-6530-4A1E-BC46-DC118D46B476}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="50">
   <si>
     <t>OP</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -35,10 +35,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>ALUOP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Branch</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -216,6 +212,18 @@
   </si>
   <si>
     <t>`1111</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>`1010</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SLT</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ALUOP[1:0]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -524,11 +532,12 @@
   <dimension ref="A1:M22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="4" max="4" width="11.5" customWidth="1"/>
     <col min="9" max="9" width="11.625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -540,42 +549,42 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>49</v>
+      </c>
+      <c r="E1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
       <c r="H1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
         <v>7</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>8</v>
       </c>
-      <c r="K1" t="s">
-        <v>9</v>
-      </c>
       <c r="L1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M1" t="s">
         <v>44</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C2">
         <v>1</v>
@@ -613,16 +622,16 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -631,7 +640,7 @@
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -640,10 +649,10 @@
         <v>0</v>
       </c>
       <c r="J3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L3">
         <v>0</v>
@@ -654,16 +663,16 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -684,7 +693,7 @@
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L4">
         <v>0</v>
@@ -695,10 +704,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C5">
         <v>1</v>
@@ -736,16 +745,16 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C6">
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -777,10 +786,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C7">
         <v>0</v>
@@ -818,10 +827,10 @@
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C8">
         <v>0</v>
@@ -859,10 +868,10 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C9">
         <v>0</v>
@@ -900,16 +909,16 @@
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B10" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -918,7 +927,7 @@
         <v>0</v>
       </c>
       <c r="G10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H10">
         <v>0</v>
@@ -927,10 +936,10 @@
         <v>0</v>
       </c>
       <c r="J10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K10" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L10">
         <v>1</v>
@@ -941,16 +950,16 @@
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -959,7 +968,7 @@
         <v>0</v>
       </c>
       <c r="G11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="H11">
         <v>0</v>
@@ -968,10 +977,10 @@
         <v>0</v>
       </c>
       <c r="J11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="K11" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="L11">
         <v>1</v>
@@ -982,48 +991,89 @@
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
+        <v>45</v>
+      </c>
+      <c r="B12" t="s">
         <v>46</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12">
+        <v>0</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0</v>
+      </c>
+      <c r="G12">
+        <v>0</v>
+      </c>
+      <c r="H12">
+        <v>0</v>
+      </c>
+      <c r="I12">
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <v>0</v>
+      </c>
+      <c r="L12">
+        <v>0</v>
+      </c>
+      <c r="M12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" t="s">
         <v>47</v>
       </c>
-      <c r="C12">
-        <v>0</v>
-      </c>
-      <c r="D12">
-        <v>0</v>
-      </c>
-      <c r="E12">
-        <v>0</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-      <c r="H12">
-        <v>0</v>
-      </c>
-      <c r="I12">
-        <v>0</v>
-      </c>
-      <c r="J12">
-        <v>0</v>
-      </c>
-      <c r="K12">
-        <v>0</v>
-      </c>
-      <c r="L12">
-        <v>0</v>
-      </c>
-      <c r="M12">
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13">
+        <v>2</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <v>0</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <v>0</v>
+      </c>
+      <c r="M13">
         <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -1032,57 +1082,57 @@
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B17" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" t="s">
         <v>31</v>
       </c>
-      <c r="C17" t="s">
-        <v>32</v>
-      </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B18" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
+        <v>31</v>
+      </c>
+      <c r="D18" t="s">
         <v>32</v>
       </c>
-      <c r="D18" t="s">
+      <c r="E18" t="s">
         <v>33</v>
-      </c>
-      <c r="E18" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B20" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" t="s">
         <v>38</v>
-      </c>
-      <c r="B22" t="s">
-        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>